<commit_message>
fixed insert upload excel in master hscode
</commit_message>
<xml_diff>
--- a/template_hscode.xlsx
+++ b/template_hscode.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>MAT CONTENT</t>
   </si>
@@ -1200,13 +1200,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="18.2857142857143" customWidth="1"/>
     <col min="2" max="2" width="18.5714285714286" customWidth="1"/>
@@ -1225,15 +1225,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>12345</v>
+        <v>67890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>